<commit_message>
read dÃata from áºexcel
</commit_message>
<xml_diff>
--- a/src/main/resources/Test data.xlsx
+++ b/src/main/resources/Test data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ancoi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\selenium\Training\vmo-fresher-selenium-hybrid\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686CEE02-9F72-4D3C-8C22-09540B578367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E60F481-BA58-425F-B9C8-6514A8FE92C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>STT</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>standard_user</t>
-  </si>
-  <si>
-    <t>sauce_secret</t>
   </si>
   <si>
     <t>Test case name</t>
@@ -72,7 +69,10 @@
     <t>Test result</t>
   </si>
   <si>
-    <t>FAILED</t>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>PASSED</t>
   </si>
 </sst>
 </file>
@@ -343,7 +343,7 @@
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -357,10 +357,10 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -369,7 +369,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="2"/>
@@ -400,15 +400,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -438,13 +440,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -474,13 +478,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -510,11 +516,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -544,7 +552,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
@@ -552,7 +560,9 @@
       <c r="D6" s="1">
         <v>123456</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -582,15 +592,17 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
         <v>123456</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>

</xml_diff>